<commit_message>
controller ready for testing?
</commit_message>
<xml_diff>
--- a/Controller/controller_V3_matlab/customer_inputs.xlsx
+++ b/Controller/controller_V3_matlab/customer_inputs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattl\Documents\Purdue\Fall 2025\ME 463\ME-463-Can-Crusher\Controller\controller_V3_matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DB08B8-CA21-4686-925F-0E17BAFD1414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6708552A-41BE-469C-B459-CD4CE2B0C6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1884" yWindow="1884" windowWidth="17964" windowHeight="11256" xr2:uid="{3A1ED538-D941-4692-8CDC-808B275BDBD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Inputs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="50" iterateDelta="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>